<commit_message>
Get info from excel,capture and save image
</commit_message>
<xml_diff>
--- a/Capture.xlsx
+++ b/Capture.xlsx
@@ -1,45 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="510" yWindow="615" windowWidth="17895" windowHeight="6345"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
   <si>
     <t>Key</t>
   </si>
   <si>
     <t>Type</t>
   </si>
+  <si>
+    <t>popup</t>
+  </si>
+  <si>
+    <t>divide</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -61,17 +69,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -361,228 +374,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="n">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="n">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="n">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="n">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="n">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="n">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="n">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="n">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="n">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="n">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="n">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="n">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="n">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="n">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="n">
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="n">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="n">
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="n">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>